<commit_message>
Refactor CO2 in constants, refactor reg count, rename classes
</commit_message>
<xml_diff>
--- a/excels/constant_raion.xlsx
+++ b/excels/constant_raion.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Antony\NSU_Education\Meteo\excels\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17340" windowHeight="9930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17340" windowHeight="9936"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -133,17 +138,17 @@
     <t>Значение</t>
   </si>
   <si>
-    <t>СО2</t>
-  </si>
-  <si>
     <t>Концентрация углекислого газа в атмосфере</t>
+  </si>
+  <si>
+    <t>CO2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,28 +652,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -679,7 +684,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -690,7 +695,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -701,7 +706,7 @@
         <v>0.28754881700000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -712,7 +717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -723,7 +728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -734,7 +739,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -745,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -756,7 +761,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18">
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -767,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18">
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -778,7 +783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -789,18 +794,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="C12" s="9">
         <v>330</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -811,7 +816,7 @@
         <v>2.6817700000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -822,7 +827,7 @@
         <v>15.3309</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
@@ -833,7 +838,7 @@
         <v>8.4072099999999992</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
@@ -844,7 +849,7 @@
         <v>3.1E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>26</v>
       </c>

</xml_diff>